<commit_message>
adjusted requirements, make scenarios, and various other things.
</commit_message>
<xml_diff>
--- a/pycirk/scenarios.xlsx
+++ b/pycirk/scenarios.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="analyse" sheetId="1" r:id="rId1"/>
@@ -10414,10 +10414,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10428,277 +10428,7 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -11336,7 +11066,7 @@
   <dimension ref="A1:IU14"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11594,7 +11324,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select category row wise" prompt="If on Z and Y it will refer to a product category being consumed_x000a_Anywhere else it should reflect the categories contained in the respective matrix e.g. W &quot;Value Added&quot;_x000a__x000a_row (i)">
           <x14:formula1>
-            <xm:f>matrix_types_for_analysis!$B$2:$B$22</xm:f>
+            <xm:f>names_categories!$C$2:$C$1618</xm:f>
           </x14:formula1>
           <xm:sqref>B5:B14</xm:sqref>
         </x14:dataValidation>
@@ -11608,8 +11338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW73"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11641,43 +11371,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="17" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42" t="s">
+      <c r="G1" s="41"/>
+      <c r="H1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42" t="s">
+      <c r="I1" s="41"/>
+      <c r="J1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="41" t="s">
+      <c r="K1" s="41"/>
+      <c r="L1" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="41"/>
+      <c r="M1" s="42"/>
       <c r="N1" s="16" t="s">
         <v>23</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42" t="s">
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="42"/>
+      <c r="S1" s="41"/>
       <c r="T1" s="43" t="s">
         <v>27</v>
       </c>
@@ -11687,7 +11417,7 @@
       <c r="X1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="42" t="s">
+      <c r="Y1" s="41" t="s">
         <v>29</v>
       </c>
     </row>
@@ -11764,7 +11494,7 @@
       <c r="X2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="42"/>
+      <c r="Y2" s="41"/>
     </row>
     <row r="3" spans="1:25" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
@@ -13924,159 +13654,159 @@
   <sheetProtection formatCells="0" formatColumns="0" insertRows="0" deleteRows="0"/>
   <autoFilter ref="A2:X10"/>
   <mergeCells count="10">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="Y1:Y2"/>
   </mergeCells>
   <conditionalFormatting sqref="X4:X463">
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:M463">
-    <cfRule type="cellIs" dxfId="54" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T74:W463">
-    <cfRule type="cellIs" dxfId="53" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X5:X39 X45:X73">
-    <cfRule type="cellIs" dxfId="52" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X40:X42">
-    <cfRule type="cellIs" dxfId="51" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:M37 H38:K39 M38:M39 L39:L42 H44:H56 H58:H73 I44:M73">
-    <cfRule type="cellIs" dxfId="50" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M40:M42 H40:K42">
-    <cfRule type="cellIs" dxfId="49" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 H3 H7 H24:H35 I3:M7 I35:M35 M8:M34 I8:K34 L9:L34 H10:H22">
-    <cfRule type="cellIs" dxfId="48" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38:L42">
-    <cfRule type="cellIs" dxfId="47" priority="10" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X53 X45:X48 X44:X47">
-    <cfRule type="cellIs" dxfId="46" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X49:X73">
-    <cfRule type="cellIs" dxfId="45" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44:M48 J53:M53">
-    <cfRule type="cellIs" dxfId="44" priority="13" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49:H56 I49:M73 H58:H73">
-    <cfRule type="cellIs" dxfId="43" priority="14" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:M43">
-    <cfRule type="cellIs" dxfId="42" priority="15" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53">
-    <cfRule type="cellIs" dxfId="41" priority="16" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="cellIs" dxfId="40" priority="17" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H68">
-    <cfRule type="cellIs" dxfId="39" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H68">
-    <cfRule type="cellIs" dxfId="38" priority="19" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="37" priority="20" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="36" priority="21" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="21" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="35" priority="22" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="22" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X4">
-    <cfRule type="cellIs" dxfId="34" priority="23" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="23" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3">
-    <cfRule type="cellIs" dxfId="33" priority="24" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="24" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L34">
-    <cfRule type="cellIs" dxfId="32" priority="25" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="25" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H34">
-    <cfRule type="cellIs" dxfId="31" priority="26" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="26" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H34">
-    <cfRule type="cellIs" dxfId="30" priority="27" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="27" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H34">
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H34">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="29" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X43:X47">
-    <cfRule type="cellIs" dxfId="27" priority="30" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="30" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14147,10 +13877,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IW1837"/>
+  <dimension ref="A1:IW1618"/>
   <sheetViews>
-    <sheetView topLeftCell="A1444" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A1580" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E1487" sqref="E1487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -33597,1554 +33327,1554 @@
         <v>3324</v>
       </c>
     </row>
-    <row r="1697" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1697" s="36" t="s">
+    <row r="1478" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1478" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1697" s="36" t="s">
+      <c r="B1478" s="36" t="s">
         <v>2962</v>
       </c>
-      <c r="C1697" s="36" t="s">
+      <c r="C1478" s="36" t="s">
         <v>2963</v>
       </c>
     </row>
-    <row r="1698" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1698" s="36" t="s">
+    <row r="1479" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1479" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1698" s="36" t="s">
+      <c r="B1479" s="36" t="s">
         <v>2964</v>
       </c>
-      <c r="C1698" s="36" t="s">
+      <c r="C1479" s="36" t="s">
         <v>2965</v>
       </c>
     </row>
-    <row r="1699" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1699" s="36" t="s">
+    <row r="1480" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1480" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1699" s="36" t="s">
+      <c r="B1480" s="36" t="s">
         <v>2962</v>
       </c>
-      <c r="C1699" s="36" t="s">
+      <c r="C1480" s="36" t="s">
         <v>2966</v>
       </c>
     </row>
-    <row r="1700" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1700" s="36" t="s">
+    <row r="1481" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1481" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1700" s="36" t="s">
+      <c r="B1481" s="36" t="s">
         <v>2962</v>
       </c>
-      <c r="C1700" s="36" t="s">
+      <c r="C1481" s="36" t="s">
         <v>2967</v>
       </c>
     </row>
-    <row r="1701" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1701" s="36" t="s">
+    <row r="1482" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1482" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1701" s="36" t="s">
+      <c r="B1482" s="36" t="s">
         <v>2968</v>
       </c>
-      <c r="C1701" s="36" t="s">
+      <c r="C1482" s="36" t="s">
         <v>2969</v>
       </c>
     </row>
-    <row r="1702" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1702" s="36" t="s">
+    <row r="1483" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1483" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1702" s="36" t="s">
+      <c r="B1483" s="36" t="s">
         <v>2970</v>
       </c>
-      <c r="C1702" s="36" t="s">
+      <c r="C1483" s="36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="1703" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1703" s="36" t="s">
+    <row r="1484" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1484" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1703" s="36" t="s">
+      <c r="B1484" s="36" t="s">
         <v>2971</v>
       </c>
-      <c r="C1703" s="36" t="s">
+      <c r="C1484" s="36" t="s">
         <v>2972</v>
       </c>
     </row>
-    <row r="1704" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1704" s="36" t="s">
+    <row r="1485" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1485" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1704" s="36" t="s">
+      <c r="B1485" s="36" t="s">
         <v>2973</v>
       </c>
-      <c r="C1704" s="36" t="s">
+      <c r="C1485" s="36" t="s">
         <v>2974</v>
       </c>
     </row>
-    <row r="1705" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1705" s="36" t="s">
+    <row r="1486" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1486" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1705" s="36" t="s">
+      <c r="B1486" s="36" t="s">
         <v>2975</v>
       </c>
-      <c r="C1705" s="36" t="s">
+      <c r="C1486" s="36" t="s">
         <v>2976</v>
       </c>
     </row>
-    <row r="1706" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1706" s="36" t="s">
+    <row r="1487" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1487" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1706" s="36" t="s">
+      <c r="B1487" s="36" t="s">
         <v>2977</v>
       </c>
-      <c r="C1706" s="36" t="s">
+      <c r="C1487" s="36" t="s">
         <v>2978</v>
       </c>
     </row>
-    <row r="1707" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1707" s="36" t="s">
+    <row r="1488" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1488" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1707" s="36" t="s">
+      <c r="B1488" s="36" t="s">
         <v>2979</v>
       </c>
-      <c r="C1707" s="36" t="s">
+      <c r="C1488" s="36" t="s">
         <v>2980</v>
       </c>
     </row>
-    <row r="1708" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1708" s="36" t="s">
+    <row r="1489" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1489" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1708" s="36" t="s">
+      <c r="B1489" s="36" t="s">
         <v>2981</v>
       </c>
-      <c r="C1708" s="36" t="s">
+      <c r="C1489" s="36" t="s">
         <v>2982</v>
       </c>
     </row>
-    <row r="1709" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1709" s="36" t="s">
+    <row r="1490" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1490" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1709" s="36" t="s">
+      <c r="B1490" s="36" t="s">
         <v>2983</v>
       </c>
-      <c r="C1709" s="36" t="s">
+      <c r="C1490" s="36" t="s">
         <v>2984</v>
       </c>
     </row>
-    <row r="1710" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1710" s="36" t="s">
+    <row r="1491" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1491" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1710" s="36" t="s">
+      <c r="B1491" s="36" t="s">
         <v>2985</v>
       </c>
-      <c r="C1710" s="36" t="s">
+      <c r="C1491" s="36" t="s">
         <v>2986</v>
       </c>
     </row>
-    <row r="1711" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1711" s="36" t="s">
+    <row r="1492" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1492" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1711" s="36" t="s">
+      <c r="B1492" s="36" t="s">
         <v>2987</v>
       </c>
-      <c r="C1711" s="36" t="s">
+      <c r="C1492" s="36" t="s">
         <v>2988</v>
       </c>
     </row>
-    <row r="1712" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1712" s="36" t="s">
+    <row r="1493" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1493" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1712" s="36" t="s">
+      <c r="B1493" s="36" t="s">
         <v>2989</v>
       </c>
-      <c r="C1712" s="36" t="s">
+      <c r="C1493" s="36" t="s">
         <v>2990</v>
       </c>
     </row>
-    <row r="1713" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1713" s="36" t="s">
+    <row r="1494" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1494" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1713" s="36" t="s">
+      <c r="B1494" s="36" t="s">
         <v>2991</v>
       </c>
-      <c r="C1713" s="36" t="s">
+      <c r="C1494" s="36" t="s">
         <v>2992</v>
       </c>
     </row>
-    <row r="1714" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1714" s="36" t="s">
+    <row r="1495" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1495" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1714" s="36" t="s">
+      <c r="B1495" s="36" t="s">
         <v>2993</v>
       </c>
-      <c r="C1714" s="36" t="s">
+      <c r="C1495" s="36" t="s">
         <v>2994</v>
       </c>
     </row>
-    <row r="1715" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1715" s="36" t="s">
+    <row r="1496" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1496" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1715" s="36" t="s">
+      <c r="B1496" s="36" t="s">
         <v>2995</v>
       </c>
-      <c r="C1715" s="36" t="s">
+      <c r="C1496" s="36" t="s">
         <v>2996</v>
       </c>
     </row>
-    <row r="1716" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1716" s="36" t="s">
+    <row r="1497" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1497" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1716" s="36" t="s">
+      <c r="B1497" s="36" t="s">
         <v>2997</v>
       </c>
-      <c r="C1716" s="36" t="s">
+      <c r="C1497" s="36" t="s">
         <v>2998</v>
       </c>
     </row>
-    <row r="1717" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1717" s="36" t="s">
+    <row r="1498" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1498" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1717" s="36" t="s">
+      <c r="B1498" s="36" t="s">
         <v>2999</v>
       </c>
-      <c r="C1717" s="36" t="s">
+      <c r="C1498" s="36" t="s">
         <v>3000</v>
       </c>
     </row>
-    <row r="1718" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1718" s="36" t="s">
+    <row r="1499" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1499" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1718" s="36" t="s">
+      <c r="B1499" s="36" t="s">
         <v>3001</v>
       </c>
-      <c r="C1718" s="36" t="s">
+      <c r="C1499" s="36" t="s">
         <v>3002</v>
       </c>
     </row>
-    <row r="1719" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1719" s="36" t="s">
+    <row r="1500" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1500" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1719" s="36" t="s">
+      <c r="B1500" s="36" t="s">
         <v>3003</v>
       </c>
-      <c r="C1719" s="36" t="s">
+      <c r="C1500" s="36" t="s">
         <v>3004</v>
       </c>
     </row>
-    <row r="1720" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1720" s="36" t="s">
+    <row r="1501" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1501" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1720" s="36" t="s">
+      <c r="B1501" s="36" t="s">
         <v>3005</v>
       </c>
-      <c r="C1720" s="36" t="s">
+      <c r="C1501" s="36" t="s">
         <v>3006</v>
       </c>
     </row>
-    <row r="1721" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1721" s="36" t="s">
+    <row r="1502" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1502" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1721" s="36" t="s">
+      <c r="B1502" s="36" t="s">
         <v>3007</v>
       </c>
-      <c r="C1721" s="36" t="s">
+      <c r="C1502" s="36" t="s">
         <v>3008</v>
       </c>
     </row>
-    <row r="1722" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1722" s="36" t="s">
+    <row r="1503" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1503" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1722" s="36" t="s">
+      <c r="B1503" s="36" t="s">
         <v>3009</v>
       </c>
-      <c r="C1722" s="36" t="s">
+      <c r="C1503" s="36" t="s">
         <v>3010</v>
       </c>
     </row>
-    <row r="1723" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1723" s="36" t="s">
+    <row r="1504" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1504" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1723" s="36" t="s">
+      <c r="B1504" s="36" t="s">
         <v>3011</v>
       </c>
-      <c r="C1723" s="36" t="s">
+      <c r="C1504" s="36" t="s">
         <v>3012</v>
       </c>
     </row>
-    <row r="1724" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1724" s="36" t="s">
+    <row r="1505" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1505" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1724" s="36" t="s">
+      <c r="B1505" s="36" t="s">
         <v>3013</v>
       </c>
-      <c r="C1724" s="36" t="s">
+      <c r="C1505" s="36" t="s">
         <v>3014</v>
       </c>
     </row>
-    <row r="1725" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1725" s="36" t="s">
+    <row r="1506" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1506" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1725" s="36" t="s">
+      <c r="B1506" s="36" t="s">
         <v>3015</v>
       </c>
-      <c r="C1725" s="36" t="s">
+      <c r="C1506" s="36" t="s">
         <v>3016</v>
       </c>
     </row>
-    <row r="1726" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1726" s="36" t="s">
+    <row r="1507" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1507" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1726" s="36" t="s">
+      <c r="B1507" s="36" t="s">
         <v>3017</v>
       </c>
-      <c r="C1726" s="36" t="s">
+      <c r="C1507" s="36" t="s">
         <v>3018</v>
       </c>
     </row>
-    <row r="1727" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1727" s="36" t="s">
+    <row r="1508" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1508" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1727" s="36" t="s">
+      <c r="B1508" s="36" t="s">
         <v>3019</v>
       </c>
-      <c r="C1727" s="36" t="s">
+      <c r="C1508" s="36" t="s">
         <v>3020</v>
       </c>
     </row>
-    <row r="1728" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1728" s="36" t="s">
+    <row r="1509" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1509" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1728" s="36" t="s">
+      <c r="B1509" s="36" t="s">
         <v>3021</v>
       </c>
-      <c r="C1728" s="36" t="s">
+      <c r="C1509" s="36" t="s">
         <v>3022</v>
       </c>
     </row>
-    <row r="1729" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1729" s="36" t="s">
+    <row r="1510" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1510" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1729" s="36" t="s">
+      <c r="B1510" s="36" t="s">
         <v>3023</v>
       </c>
-      <c r="C1729" s="36" t="s">
+      <c r="C1510" s="36" t="s">
         <v>3024</v>
       </c>
     </row>
-    <row r="1730" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1730" s="36" t="s">
+    <row r="1511" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1511" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1730" s="36" t="s">
+      <c r="B1511" s="36" t="s">
         <v>3025</v>
       </c>
-      <c r="C1730" s="36" t="s">
+      <c r="C1511" s="36" t="s">
         <v>3026</v>
       </c>
     </row>
-    <row r="1731" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1731" s="36" t="s">
+    <row r="1512" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1512" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1731" s="36" t="s">
+      <c r="B1512" s="36" t="s">
         <v>3027</v>
       </c>
-      <c r="C1731" s="36" t="s">
+      <c r="C1512" s="36" t="s">
         <v>3028</v>
       </c>
     </row>
-    <row r="1732" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1732" s="36" t="s">
+    <row r="1513" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1513" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1732" s="36" t="s">
+      <c r="B1513" s="36" t="s">
         <v>3029</v>
       </c>
-      <c r="C1732" s="36" t="s">
+      <c r="C1513" s="36" t="s">
         <v>3030</v>
       </c>
     </row>
-    <row r="1733" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1733" s="36" t="s">
+    <row r="1514" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1514" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1733" s="36" t="s">
+      <c r="B1514" s="36" t="s">
         <v>3031</v>
       </c>
-      <c r="C1733" s="36" t="s">
+      <c r="C1514" s="36" t="s">
         <v>3032</v>
       </c>
     </row>
-    <row r="1734" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1734" s="36" t="s">
+    <row r="1515" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1515" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1734" s="36" t="s">
+      <c r="B1515" s="36" t="s">
         <v>3033</v>
       </c>
-      <c r="C1734" s="36" t="s">
+      <c r="C1515" s="36" t="s">
         <v>3034</v>
       </c>
     </row>
-    <row r="1735" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1735" s="36" t="s">
+    <row r="1516" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1516" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1735" s="36" t="s">
+      <c r="B1516" s="36" t="s">
         <v>3035</v>
       </c>
-      <c r="C1735" s="36" t="s">
+      <c r="C1516" s="36" t="s">
         <v>3036</v>
       </c>
     </row>
-    <row r="1736" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1736" s="36" t="s">
+    <row r="1517" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1517" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1736" s="36" t="s">
+      <c r="B1517" s="36" t="s">
         <v>3037</v>
       </c>
-      <c r="C1736" s="36" t="s">
+      <c r="C1517" s="36" t="s">
         <v>3038</v>
       </c>
     </row>
-    <row r="1737" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1737" s="36" t="s">
+    <row r="1518" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1518" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1737" s="36" t="s">
+      <c r="B1518" s="36" t="s">
         <v>3039</v>
       </c>
-      <c r="C1737" s="36" t="s">
+      <c r="C1518" s="36" t="s">
         <v>3040</v>
       </c>
     </row>
-    <row r="1738" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1738" s="36" t="s">
+    <row r="1519" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1519" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1738" s="36" t="s">
+      <c r="B1519" s="36" t="s">
         <v>3041</v>
       </c>
-      <c r="C1738" s="36" t="s">
+      <c r="C1519" s="36" t="s">
         <v>3042</v>
       </c>
     </row>
-    <row r="1739" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1739" s="36" t="s">
+    <row r="1520" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1520" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1739" s="36" t="s">
+      <c r="B1520" s="36" t="s">
         <v>3043</v>
       </c>
-      <c r="C1739" s="36" t="s">
+      <c r="C1520" s="36" t="s">
         <v>3044</v>
       </c>
     </row>
-    <row r="1740" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1740" s="36" t="s">
+    <row r="1521" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1521" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1740" s="36" t="s">
+      <c r="B1521" s="36" t="s">
         <v>3045</v>
       </c>
-      <c r="C1740" s="36" t="s">
+      <c r="C1521" s="36" t="s">
         <v>3046</v>
       </c>
     </row>
-    <row r="1741" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1741" s="36" t="s">
+    <row r="1522" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1522" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1741" s="36" t="s">
+      <c r="B1522" s="36" t="s">
         <v>3047</v>
       </c>
-      <c r="C1741" s="36" t="s">
+      <c r="C1522" s="36" t="s">
         <v>3048</v>
       </c>
     </row>
-    <row r="1742" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1742" s="36" t="s">
+    <row r="1523" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1523" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1742" s="36" t="s">
+      <c r="B1523" s="36" t="s">
         <v>3049</v>
       </c>
-      <c r="C1742" s="36" t="s">
+      <c r="C1523" s="36" t="s">
         <v>3050</v>
       </c>
     </row>
-    <row r="1743" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1743" s="36" t="s">
+    <row r="1524" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1524" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1743" s="36" t="s">
+      <c r="B1524" s="36" t="s">
         <v>3051</v>
       </c>
-      <c r="C1743" s="36" t="s">
+      <c r="C1524" s="36" t="s">
         <v>3052</v>
       </c>
     </row>
-    <row r="1744" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1744" s="36" t="s">
+    <row r="1525" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1525" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1744" s="36" t="s">
+      <c r="B1525" s="36" t="s">
         <v>3053</v>
       </c>
-      <c r="C1744" s="36" t="s">
+      <c r="C1525" s="36" t="s">
         <v>3054</v>
       </c>
     </row>
-    <row r="1745" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1745" s="36" t="s">
+    <row r="1526" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1526" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1745" s="36" t="s">
+      <c r="B1526" s="36" t="s">
         <v>3055</v>
       </c>
-      <c r="C1745" s="36" t="s">
+      <c r="C1526" s="36" t="s">
         <v>3056</v>
       </c>
     </row>
-    <row r="1746" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1746" s="36" t="s">
+    <row r="1527" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1527" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1746" s="36" t="s">
+      <c r="B1527" s="36" t="s">
         <v>3057</v>
       </c>
-      <c r="C1746" s="36" t="s">
+      <c r="C1527" s="36" t="s">
         <v>3058</v>
       </c>
     </row>
-    <row r="1747" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1747" s="36" t="s">
+    <row r="1528" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1528" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1747" s="36" t="s">
+      <c r="B1528" s="36" t="s">
         <v>3059</v>
       </c>
-      <c r="C1747" s="36" t="s">
+      <c r="C1528" s="36" t="s">
         <v>3060</v>
       </c>
     </row>
-    <row r="1748" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1748" s="36" t="s">
+    <row r="1529" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1529" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1748" s="36" t="s">
+      <c r="B1529" s="36" t="s">
         <v>3061</v>
       </c>
-      <c r="C1748" s="36" t="s">
+      <c r="C1529" s="36" t="s">
         <v>3062</v>
       </c>
     </row>
-    <row r="1749" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1749" s="36" t="s">
+    <row r="1530" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1530" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1749" s="36" t="s">
+      <c r="B1530" s="36" t="s">
         <v>3063</v>
       </c>
-      <c r="C1749" s="36" t="s">
+      <c r="C1530" s="36" t="s">
         <v>3064</v>
       </c>
     </row>
-    <row r="1750" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1750" s="36" t="s">
+    <row r="1531" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1531" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1750" s="36" t="s">
+      <c r="B1531" s="36" t="s">
         <v>3065</v>
       </c>
-      <c r="C1750" s="36" t="s">
+      <c r="C1531" s="36" t="s">
         <v>3066</v>
       </c>
     </row>
-    <row r="1751" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1751" s="36" t="s">
+    <row r="1532" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1532" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1751" s="36" t="s">
+      <c r="B1532" s="36" t="s">
         <v>3067</v>
       </c>
-      <c r="C1751" s="36" t="s">
+      <c r="C1532" s="36" t="s">
         <v>3068</v>
       </c>
     </row>
-    <row r="1752" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1752" s="36" t="s">
+    <row r="1533" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1533" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1752" s="36" t="s">
+      <c r="B1533" s="36" t="s">
         <v>3069</v>
       </c>
-      <c r="C1752" s="36" t="s">
+      <c r="C1533" s="36" t="s">
         <v>3069</v>
       </c>
     </row>
-    <row r="1753" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1753" s="36" t="s">
+    <row r="1534" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1534" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1753" s="36" t="s">
+      <c r="B1534" s="36" t="s">
         <v>3070</v>
       </c>
-      <c r="C1753" s="36" t="s">
+      <c r="C1534" s="36" t="s">
         <v>3070</v>
       </c>
     </row>
-    <row r="1754" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1754" s="36" t="s">
+    <row r="1535" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1535" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1754" s="36" t="s">
+      <c r="B1535" s="36" t="s">
         <v>3071</v>
       </c>
-      <c r="C1754" s="36" t="s">
+      <c r="C1535" s="36" t="s">
         <v>3071</v>
       </c>
     </row>
-    <row r="1755" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1755" s="36" t="s">
+    <row r="1536" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1536" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1755" s="36" t="s">
+      <c r="B1536" s="36" t="s">
         <v>3072</v>
       </c>
-      <c r="C1755" s="36" t="s">
+      <c r="C1536" s="36" t="s">
         <v>3072</v>
       </c>
     </row>
-    <row r="1756" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1756" s="36" t="s">
+    <row r="1537" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1537" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1756" s="36" t="s">
+      <c r="B1537" s="36" t="s">
         <v>3073</v>
       </c>
-      <c r="C1756" s="36" t="s">
+      <c r="C1537" s="36" t="s">
         <v>3073</v>
       </c>
     </row>
-    <row r="1757" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1757" s="36" t="s">
+    <row r="1538" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1538" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1757" s="36" t="s">
+      <c r="B1538" s="36" t="s">
         <v>3074</v>
       </c>
-      <c r="C1757" s="36" t="s">
+      <c r="C1538" s="36" t="s">
         <v>3074</v>
       </c>
     </row>
-    <row r="1758" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1758" s="36" t="s">
+    <row r="1539" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1539" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1758" s="36" t="s">
+      <c r="B1539" s="36" t="s">
         <v>3075</v>
       </c>
-      <c r="C1758" s="36" t="s">
+      <c r="C1539" s="36" t="s">
         <v>3075</v>
       </c>
     </row>
-    <row r="1759" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1759" s="36" t="s">
+    <row r="1540" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1540" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1759" s="36" t="s">
+      <c r="B1540" s="36" t="s">
         <v>3076</v>
       </c>
-      <c r="C1759" s="36" t="s">
+      <c r="C1540" s="36" t="s">
         <v>3076</v>
       </c>
     </row>
-    <row r="1760" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1760" s="36" t="s">
+    <row r="1541" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1541" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1760" s="36" t="s">
+      <c r="B1541" s="36" t="s">
         <v>3077</v>
       </c>
-      <c r="C1760" s="36" t="s">
+      <c r="C1541" s="36" t="s">
         <v>3077</v>
       </c>
     </row>
-    <row r="1761" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1761" s="36" t="s">
+    <row r="1542" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1542" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1761" s="36" t="s">
+      <c r="B1542" s="36" t="s">
         <v>3078</v>
       </c>
-      <c r="C1761" s="36" t="s">
+      <c r="C1542" s="36" t="s">
         <v>3078</v>
       </c>
     </row>
-    <row r="1762" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1762" s="36" t="s">
+    <row r="1543" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1543" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1762" s="36" t="s">
+      <c r="B1543" s="36" t="s">
         <v>3079</v>
       </c>
-      <c r="C1762" s="36" t="s">
+      <c r="C1543" s="36" t="s">
         <v>3079</v>
       </c>
     </row>
-    <row r="1763" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1763" s="36" t="s">
+    <row r="1544" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1544" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1763" s="36" t="s">
+      <c r="B1544" s="36" t="s">
         <v>3080</v>
       </c>
-      <c r="C1763" s="36" t="s">
+      <c r="C1544" s="36" t="s">
         <v>3080</v>
       </c>
     </row>
-    <row r="1764" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1764" s="36" t="s">
+    <row r="1545" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1545" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1764" s="36" t="s">
+      <c r="B1545" s="36" t="s">
         <v>3081</v>
       </c>
-      <c r="C1764" s="36" t="s">
+      <c r="C1545" s="36" t="s">
         <v>3081</v>
       </c>
     </row>
-    <row r="1765" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1765" s="36" t="s">
+    <row r="1546" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1546" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1765" s="36" t="s">
+      <c r="B1546" s="36" t="s">
         <v>3082</v>
       </c>
-      <c r="C1765" s="36" t="s">
+      <c r="C1546" s="36" t="s">
         <v>3082</v>
       </c>
     </row>
-    <row r="1766" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1766" s="36" t="s">
+    <row r="1547" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1547" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1766" s="36" t="s">
+      <c r="B1547" s="36" t="s">
         <v>3083</v>
       </c>
-      <c r="C1766" s="36" t="s">
+      <c r="C1547" s="36" t="s">
         <v>3083</v>
       </c>
     </row>
-    <row r="1767" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1767" s="36" t="s">
+    <row r="1548" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1548" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1767" s="36" t="s">
+      <c r="B1548" s="36" t="s">
         <v>3084</v>
       </c>
-      <c r="C1767" s="36" t="s">
+      <c r="C1548" s="36" t="s">
         <v>3084</v>
       </c>
     </row>
-    <row r="1768" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1768" s="36" t="s">
+    <row r="1549" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1549" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1768" s="36" t="s">
+      <c r="B1549" s="36" t="s">
         <v>3085</v>
       </c>
-      <c r="C1768" s="36" t="s">
+      <c r="C1549" s="36" t="s">
         <v>3085</v>
       </c>
     </row>
-    <row r="1769" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1769" s="36" t="s">
+    <row r="1550" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1550" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1769" s="36" t="s">
+      <c r="B1550" s="36" t="s">
         <v>3086</v>
       </c>
-      <c r="C1769" s="36" t="s">
+      <c r="C1550" s="36" t="s">
         <v>3086</v>
       </c>
     </row>
-    <row r="1770" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1770" s="36" t="s">
+    <row r="1551" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1551" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1770" s="36" t="s">
+      <c r="B1551" s="36" t="s">
         <v>3087</v>
       </c>
-      <c r="C1770" s="36" t="s">
+      <c r="C1551" s="36" t="s">
         <v>3087</v>
       </c>
     </row>
-    <row r="1771" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1771" s="36" t="s">
+    <row r="1552" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1552" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1771" s="36" t="s">
+      <c r="B1552" s="36" t="s">
         <v>3088</v>
       </c>
-      <c r="C1771" s="36" t="s">
+      <c r="C1552" s="36" t="s">
         <v>3088</v>
       </c>
     </row>
-    <row r="1772" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1772" s="36" t="s">
+    <row r="1553" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1553" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1772" s="36" t="s">
+      <c r="B1553" s="36" t="s">
         <v>3089</v>
       </c>
-      <c r="C1772" s="36" t="s">
+      <c r="C1553" s="36" t="s">
         <v>3089</v>
       </c>
     </row>
-    <row r="1773" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1773" s="36" t="s">
+    <row r="1554" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1554" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1773" s="36" t="s">
+      <c r="B1554" s="36" t="s">
         <v>3090</v>
       </c>
-      <c r="C1773" s="36" t="s">
+      <c r="C1554" s="36" t="s">
         <v>3090</v>
       </c>
     </row>
-    <row r="1774" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1774" s="36" t="s">
+    <row r="1555" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1555" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1774" s="36" t="s">
+      <c r="B1555" s="36" t="s">
         <v>3091</v>
       </c>
-      <c r="C1774" s="36" t="s">
+      <c r="C1555" s="36" t="s">
         <v>3091</v>
       </c>
     </row>
-    <row r="1775" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1775" s="36" t="s">
+    <row r="1556" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1556" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1775" s="36" t="s">
+      <c r="B1556" s="36" t="s">
         <v>3092</v>
       </c>
-      <c r="C1775" s="36" t="s">
+      <c r="C1556" s="36" t="s">
         <v>3092</v>
       </c>
     </row>
-    <row r="1776" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1776" s="36" t="s">
+    <row r="1557" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1557" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1776" s="36" t="s">
+      <c r="B1557" s="36" t="s">
         <v>3093</v>
       </c>
-      <c r="C1776" s="36" t="s">
+      <c r="C1557" s="36" t="s">
         <v>3093</v>
       </c>
     </row>
-    <row r="1777" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1777" s="36" t="s">
+    <row r="1558" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1558" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1777" s="36" t="s">
+      <c r="B1558" s="36" t="s">
         <v>3094</v>
       </c>
-      <c r="C1777" s="36" t="s">
+      <c r="C1558" s="36" t="s">
         <v>3094</v>
       </c>
     </row>
-    <row r="1778" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1778" s="36" t="s">
+    <row r="1559" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1559" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1778" s="36" t="s">
+      <c r="B1559" s="36" t="s">
         <v>3095</v>
       </c>
-      <c r="C1778" s="36" t="s">
+      <c r="C1559" s="36" t="s">
         <v>3095</v>
       </c>
     </row>
-    <row r="1779" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1779" s="36" t="s">
+    <row r="1560" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1560" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1779" s="36" t="s">
+      <c r="B1560" s="36" t="s">
         <v>3096</v>
       </c>
-      <c r="C1779" s="36" t="s">
+      <c r="C1560" s="36" t="s">
         <v>3096</v>
       </c>
     </row>
-    <row r="1780" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1780" s="36" t="s">
+    <row r="1561" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1561" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1780" s="36" t="s">
+      <c r="B1561" s="36" t="s">
         <v>3097</v>
       </c>
-      <c r="C1780" s="36" t="s">
+      <c r="C1561" s="36" t="s">
         <v>3097</v>
       </c>
     </row>
-    <row r="1781" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1781" s="36" t="s">
+    <row r="1562" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1562" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1781" s="36" t="s">
+      <c r="B1562" s="36" t="s">
         <v>3098</v>
       </c>
-      <c r="C1781" s="36" t="s">
+      <c r="C1562" s="36" t="s">
         <v>3098</v>
       </c>
     </row>
-    <row r="1782" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1782" s="36" t="s">
+    <row r="1563" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1563" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1782" s="36" t="s">
+      <c r="B1563" s="36" t="s">
         <v>3099</v>
       </c>
-      <c r="C1782" s="36" t="s">
+      <c r="C1563" s="36" t="s">
         <v>3099</v>
       </c>
     </row>
-    <row r="1783" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1783" s="36" t="s">
+    <row r="1564" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1564" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1783" s="36" t="s">
+      <c r="B1564" s="36" t="s">
         <v>3100</v>
       </c>
-      <c r="C1783" s="36" t="s">
+      <c r="C1564" s="36" t="s">
         <v>3100</v>
       </c>
     </row>
-    <row r="1784" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1784" s="36" t="s">
+    <row r="1565" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1565" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1784" s="36" t="s">
+      <c r="B1565" s="36" t="s">
         <v>3101</v>
       </c>
-      <c r="C1784" s="36" t="s">
+      <c r="C1565" s="36" t="s">
         <v>3101</v>
       </c>
     </row>
-    <row r="1785" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1785" s="36" t="s">
+    <row r="1566" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1566" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1785" s="36" t="s">
+      <c r="B1566" s="36" t="s">
         <v>3102</v>
       </c>
-      <c r="C1785" s="36" t="s">
+      <c r="C1566" s="36" t="s">
         <v>3102</v>
       </c>
     </row>
-    <row r="1786" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1786" s="36" t="s">
+    <row r="1567" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1567" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1786" s="36" t="s">
+      <c r="B1567" s="36" t="s">
         <v>3103</v>
       </c>
-      <c r="C1786" s="36" t="s">
+      <c r="C1567" s="36" t="s">
         <v>3103</v>
       </c>
     </row>
-    <row r="1787" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1787" s="36" t="s">
+    <row r="1568" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1568" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1787" s="36" t="s">
+      <c r="B1568" s="36" t="s">
         <v>3104</v>
       </c>
-      <c r="C1787" s="36" t="s">
+      <c r="C1568" s="36" t="s">
         <v>3104</v>
       </c>
     </row>
-    <row r="1788" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1788" s="36" t="s">
+    <row r="1569" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1569" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1788" s="36" t="s">
+      <c r="B1569" s="36" t="s">
         <v>3105</v>
       </c>
-      <c r="C1788" s="36" t="s">
+      <c r="C1569" s="36" t="s">
         <v>3105</v>
       </c>
     </row>
-    <row r="1789" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1789" s="36" t="s">
+    <row r="1570" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1570" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1789" s="36" t="s">
+      <c r="B1570" s="36" t="s">
         <v>3106</v>
       </c>
-      <c r="C1789" s="36" t="s">
+      <c r="C1570" s="36" t="s">
         <v>3107</v>
       </c>
     </row>
-    <row r="1790" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1790" s="36" t="s">
+    <row r="1571" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1571" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1790" s="36" t="s">
+      <c r="B1571" s="36" t="s">
         <v>3108</v>
       </c>
-      <c r="C1790" s="36" t="s">
+      <c r="C1571" s="36" t="s">
         <v>3109</v>
       </c>
     </row>
-    <row r="1791" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1791" s="36" t="s">
+    <row r="1572" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1572" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1791" s="36" t="s">
+      <c r="B1572" s="36" t="s">
         <v>3110</v>
       </c>
-      <c r="C1791" s="36" t="s">
+      <c r="C1572" s="36" t="s">
         <v>3111</v>
       </c>
     </row>
-    <row r="1792" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1792" s="36" t="s">
+    <row r="1573" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1573" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1792" s="36" t="s">
+      <c r="B1573" s="36" t="s">
         <v>3112</v>
       </c>
-      <c r="C1792" s="36" t="s">
+      <c r="C1573" s="36" t="s">
         <v>3113</v>
       </c>
     </row>
-    <row r="1793" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1793" s="36" t="s">
+    <row r="1574" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1574" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1793" s="36" t="s">
+      <c r="B1574" s="36" t="s">
         <v>3108</v>
       </c>
-      <c r="C1793" s="36" t="s">
+      <c r="C1574" s="36" t="s">
         <v>3114</v>
       </c>
     </row>
-    <row r="1794" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1794" s="36" t="s">
+    <row r="1575" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1575" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1794" s="36" t="s">
+      <c r="B1575" s="36" t="s">
         <v>3115</v>
       </c>
-      <c r="C1794" s="36" t="s">
+      <c r="C1575" s="36" t="s">
         <v>3116</v>
       </c>
     </row>
-    <row r="1795" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1795" s="36" t="s">
+    <row r="1576" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1576" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1795" s="36" t="s">
+      <c r="B1576" s="36" t="s">
         <v>3115</v>
       </c>
-      <c r="C1795" s="36" t="s">
+      <c r="C1576" s="36" t="s">
         <v>3117</v>
       </c>
     </row>
-    <row r="1796" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1796" s="36" t="s">
+    <row r="1577" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1577" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1796" s="36" t="s">
+      <c r="B1577" s="36" t="s">
         <v>3108</v>
       </c>
-      <c r="C1796" s="36" t="s">
+      <c r="C1577" s="36" t="s">
         <v>3118</v>
       </c>
     </row>
-    <row r="1797" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1797" s="36" t="s">
+    <row r="1578" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1578" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1797" s="36" t="s">
+      <c r="B1578" s="36" t="s">
         <v>3108</v>
       </c>
-      <c r="C1797" s="36" t="s">
+      <c r="C1578" s="36" t="s">
         <v>3119</v>
       </c>
     </row>
-    <row r="1798" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1798" s="36" t="s">
+    <row r="1579" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1579" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1798" s="36" t="s">
+      <c r="B1579" s="36" t="s">
         <v>3120</v>
       </c>
-      <c r="C1798" s="36" t="s">
+      <c r="C1579" s="36" t="s">
         <v>3121</v>
       </c>
     </row>
-    <row r="1799" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1799" s="36" t="s">
+    <row r="1580" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1580" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1799" s="36" t="s">
+      <c r="B1580" s="36" t="s">
         <v>3108</v>
       </c>
-      <c r="C1799" s="36" t="s">
+      <c r="C1580" s="36" t="s">
         <v>3122</v>
       </c>
     </row>
-    <row r="1800" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1800" s="36" t="s">
+    <row r="1581" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1581" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1800" s="36" t="s">
+      <c r="B1581" s="36" t="s">
         <v>3123</v>
       </c>
-      <c r="C1800" s="36" t="s">
+      <c r="C1581" s="36" t="s">
         <v>3124</v>
       </c>
     </row>
-    <row r="1801" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1801" s="36" t="s">
+    <row r="1582" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1582" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1801" s="36" t="s">
+      <c r="B1582" s="36" t="s">
         <v>3123</v>
       </c>
-      <c r="C1801" s="36" t="s">
+      <c r="C1582" s="36" t="s">
         <v>3125</v>
       </c>
     </row>
-    <row r="1802" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1802" s="36" t="s">
+    <row r="1583" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1583" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1802" s="36" t="s">
+      <c r="B1583" s="36" t="s">
         <v>3108</v>
       </c>
-      <c r="C1802" s="36" t="s">
+      <c r="C1583" s="36" t="s">
         <v>3126</v>
       </c>
     </row>
-    <row r="1803" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1803" s="36" t="s">
+    <row r="1584" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1584" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1803" s="36" t="s">
+      <c r="B1584" s="36" t="s">
         <v>3110</v>
       </c>
-      <c r="C1803" s="36" t="s">
+      <c r="C1584" s="36" t="s">
         <v>3127</v>
       </c>
     </row>
-    <row r="1804" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1804" s="36" t="s">
+    <row r="1585" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1585" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1804" s="36" t="s">
+      <c r="B1585" s="36" t="s">
         <v>3128</v>
       </c>
-      <c r="C1804" s="36" t="s">
+      <c r="C1585" s="36" t="s">
         <v>3129</v>
       </c>
     </row>
-    <row r="1805" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1805" s="36" t="s">
+    <row r="1586" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1586" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1805" s="36" t="s">
+      <c r="B1586" s="36" t="s">
         <v>3108</v>
       </c>
-      <c r="C1805" s="36" t="s">
+      <c r="C1586" s="36" t="s">
         <v>3130</v>
       </c>
     </row>
-    <row r="1806" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1806" s="36" t="s">
+    <row r="1587" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1587" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1806" s="36" t="s">
+      <c r="B1587" s="36" t="s">
         <v>3131</v>
       </c>
-      <c r="C1806" s="36" t="s">
+      <c r="C1587" s="36" t="s">
         <v>3132</v>
       </c>
     </row>
-    <row r="1807" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1807" s="36" t="s">
+    <row r="1588" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1588" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1807" s="36" t="s">
+      <c r="B1588" s="36" t="s">
         <v>3133</v>
       </c>
-      <c r="C1807" s="36" t="s">
+      <c r="C1588" s="36" t="s">
         <v>3134</v>
       </c>
     </row>
-    <row r="1808" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1808" s="36" t="s">
+    <row r="1589" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1589" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1808" s="36" t="s">
+      <c r="B1589" s="36" t="s">
         <v>3131</v>
       </c>
-      <c r="C1808" s="36" t="s">
+      <c r="C1589" s="36" t="s">
         <v>3135</v>
       </c>
     </row>
-    <row r="1809" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1809" s="36" t="s">
+    <row r="1590" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1590" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1809" s="36" t="s">
+      <c r="B1590" s="36" t="s">
         <v>3110</v>
       </c>
-      <c r="C1809" s="36" t="s">
+      <c r="C1590" s="36" t="s">
         <v>3136</v>
       </c>
     </row>
-    <row r="1810" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1810" s="36" t="s">
+    <row r="1591" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1591" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1810" s="36" t="s">
+      <c r="B1591" s="36" t="s">
         <v>3110</v>
       </c>
-      <c r="C1810" s="36" t="s">
+      <c r="C1591" s="36" t="s">
         <v>3137</v>
       </c>
     </row>
-    <row r="1811" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1811" s="36" t="s">
+    <row r="1592" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1592" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1811" s="36" t="s">
+      <c r="B1592" s="36" t="s">
         <v>3110</v>
       </c>
-      <c r="C1811" s="36" t="s">
+      <c r="C1592" s="36" t="s">
         <v>3138</v>
       </c>
     </row>
-    <row r="1812" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1812" s="36" t="s">
+    <row r="1593" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1593" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1812" s="36" t="s">
+      <c r="B1593" s="36" t="s">
         <v>3139</v>
       </c>
-      <c r="C1812" s="36" t="s">
+      <c r="C1593" s="36" t="s">
         <v>3140</v>
       </c>
     </row>
-    <row r="1813" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1813" s="36" t="s">
+    <row r="1594" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1594" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1813" s="36" t="s">
+      <c r="B1594" s="36" t="s">
         <v>3110</v>
       </c>
-      <c r="C1813" s="36" t="s">
+      <c r="C1594" s="36" t="s">
         <v>3141</v>
       </c>
     </row>
-    <row r="1814" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1814" s="36" t="s">
+    <row r="1595" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1595" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1814" s="36" t="s">
+      <c r="B1595" s="36" t="s">
         <v>3123</v>
       </c>
-      <c r="C1814" s="36" t="s">
+      <c r="C1595" s="36" t="s">
         <v>3142</v>
       </c>
     </row>
-    <row r="1815" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1815" s="36" t="s">
+    <row r="1596" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1596" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1815" s="36" t="s">
+      <c r="B1596" s="36" t="s">
         <v>3143</v>
       </c>
-      <c r="C1815" s="36" t="s">
+      <c r="C1596" s="36" t="s">
         <v>3144</v>
       </c>
     </row>
-    <row r="1816" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1816" s="36" t="s">
+    <row r="1597" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1597" s="36" t="s">
         <v>2961</v>
       </c>
-      <c r="B1816" s="36" t="s">
+      <c r="B1597" s="36" t="s">
         <v>3145</v>
       </c>
-      <c r="C1816" s="36" t="s">
+      <c r="C1597" s="36" t="s">
         <v>3146</v>
       </c>
     </row>
-    <row r="1817" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1817" s="36" t="s">
+    <row r="1598" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1598" s="36" t="s">
         <v>3147</v>
       </c>
-      <c r="B1817" s="36" t="s">
+      <c r="B1598" s="36" t="s">
         <v>3148</v>
       </c>
-      <c r="C1817" s="36" t="s">
-        <v>3148</v>
-      </c>
-    </row>
-    <row r="1818" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1818" s="36" t="s">
+      <c r="C1598" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1599" s="36" t="s">
         <v>3147</v>
       </c>
-      <c r="B1818" s="36" t="s">
+      <c r="B1599" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C1818" s="36" t="s">
+      <c r="C1599" s="36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="1819" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1819" s="36" t="s">
+    <row r="1600" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1600" s="36" t="s">
         <v>3147</v>
       </c>
-      <c r="B1819" s="36" t="s">
+      <c r="B1600" s="36" t="s">
         <v>3149</v>
       </c>
-      <c r="C1819" s="36" t="s">
+      <c r="C1600" s="36" t="s">
         <v>3149</v>
       </c>
     </row>
-    <row r="1820" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1820" s="36" t="s">
+    <row r="1601" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1601" s="36" t="s">
         <v>3150</v>
       </c>
-      <c r="B1820" s="36" t="s">
+      <c r="B1601" s="36" t="s">
         <v>3151</v>
       </c>
-      <c r="C1820" s="36" t="s">
+      <c r="C1601" s="36" t="s">
         <v>3151</v>
       </c>
     </row>
-    <row r="1821" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1821" s="36" t="s">
+    <row r="1602" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1602" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1821" s="36" t="s">
+      <c r="B1602" s="36" t="s">
         <v>3153</v>
       </c>
-      <c r="C1821" s="36" t="s">
+      <c r="C1602" s="36" t="s">
         <v>3153</v>
       </c>
     </row>
-    <row r="1822" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1822" s="36" t="s">
+    <row r="1603" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1603" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1822" s="36" t="s">
+      <c r="B1603" s="36" t="s">
         <v>3154</v>
       </c>
-      <c r="C1822" s="36" t="s">
+      <c r="C1603" s="36" t="s">
         <v>3154</v>
       </c>
     </row>
-    <row r="1823" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1823" s="36" t="s">
+    <row r="1604" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1604" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1823" s="36" t="s">
+      <c r="B1604" s="36" t="s">
         <v>3155</v>
       </c>
-      <c r="C1823" s="36" t="s">
+      <c r="C1604" s="36" t="s">
         <v>3155</v>
       </c>
     </row>
-    <row r="1824" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1824" s="36" t="s">
+    <row r="1605" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1605" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1824" s="36" t="s">
+      <c r="B1605" s="36" t="s">
         <v>3156</v>
       </c>
-      <c r="C1824" s="36" t="s">
+      <c r="C1605" s="36" t="s">
         <v>3156</v>
       </c>
     </row>
-    <row r="1825" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1825" s="36" t="s">
+    <row r="1606" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1606" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1825" s="36" t="s">
+      <c r="B1606" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C1825" s="36" t="s">
+      <c r="C1606" s="36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="1826" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1826" s="36" t="s">
+    <row r="1607" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1607" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1826" s="36" t="s">
+      <c r="B1607" s="36" t="s">
         <v>3157</v>
       </c>
-      <c r="C1826" s="36" t="s">
+      <c r="C1607" s="36" t="s">
         <v>3157</v>
       </c>
     </row>
-    <row r="1827" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1827" s="36" t="s">
+    <row r="1608" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1608" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1827" s="36" t="s">
+      <c r="B1608" s="36" t="s">
         <v>3158</v>
       </c>
-      <c r="C1827" s="36" t="s">
+      <c r="C1608" s="36" t="s">
         <v>3158</v>
       </c>
     </row>
-    <row r="1828" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1828" s="36" t="s">
+    <row r="1609" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1609" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1828" s="36" t="s">
+      <c r="B1609" s="36" t="s">
         <v>3159</v>
       </c>
-      <c r="C1828" s="36" t="s">
+      <c r="C1609" s="36" t="s">
         <v>3159</v>
       </c>
     </row>
-    <row r="1829" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1829" s="36" t="s">
+    <row r="1610" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1610" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1829" s="36" t="s">
+      <c r="B1610" s="36" t="s">
         <v>3160</v>
       </c>
-      <c r="C1829" s="36" t="s">
+      <c r="C1610" s="36" t="s">
         <v>3160</v>
       </c>
     </row>
-    <row r="1830" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1830" s="36" t="s">
+    <row r="1611" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1611" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1830" s="36" t="s">
+      <c r="B1611" s="36" t="s">
         <v>3161</v>
       </c>
-      <c r="C1830" s="36" t="s">
+      <c r="C1611" s="36" t="s">
         <v>3161</v>
       </c>
     </row>
-    <row r="1831" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1831" s="36" t="s">
+    <row r="1612" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1612" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1831" s="36" t="s">
+      <c r="B1612" s="36" t="s">
         <v>3162</v>
       </c>
-      <c r="C1831" s="36" t="s">
+      <c r="C1612" s="36" t="s">
         <v>3162</v>
       </c>
     </row>
-    <row r="1832" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1832" s="36" t="s">
+    <row r="1613" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1613" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1832" s="36" t="s">
+      <c r="B1613" s="36" t="s">
         <v>3163</v>
       </c>
-      <c r="C1832" s="36" t="s">
+      <c r="C1613" s="36" t="s">
         <v>3163</v>
       </c>
     </row>
-    <row r="1833" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1833" s="36" t="s">
+    <row r="1614" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1614" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1833" s="36" t="s">
+      <c r="B1614" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C1833" s="36" t="s">
+      <c r="C1614" s="36" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="1834" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1834" s="36" t="s">
+    <row r="1615" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1615" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1834" s="36" t="s">
+      <c r="B1615" s="36" t="s">
         <v>3164</v>
       </c>
-      <c r="C1834" s="36" t="s">
+      <c r="C1615" s="36" t="s">
         <v>3164</v>
       </c>
     </row>
-    <row r="1835" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1835" s="36" t="s">
+    <row r="1616" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1616" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1835" s="36" t="s">
+      <c r="B1616" s="36" t="s">
         <v>3165</v>
       </c>
-      <c r="C1835" s="36" t="s">
+      <c r="C1616" s="36" t="s">
         <v>3165</v>
       </c>
     </row>
-    <row r="1836" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1836" s="36" t="s">
+    <row r="1617" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1617" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1836" s="36" t="s">
+      <c r="B1617" s="36" t="s">
         <v>3166</v>
       </c>
-      <c r="C1836" s="36" t="s">
+      <c r="C1617" s="36" t="s">
         <v>3166</v>
       </c>
     </row>
-    <row r="1837" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1837" s="36" t="s">
+    <row r="1618" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1618" s="36" t="s">
         <v>3152</v>
       </c>
-      <c r="B1837" s="36" t="s">
+      <c r="B1618" s="36" t="s">
         <v>3167</v>
       </c>
-      <c r="C1837" s="36" t="s">
+      <c r="C1618" s="36" t="s">
         <v>3167</v>
       </c>
     </row>
@@ -35536,7 +35266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>

</xml_diff>